<commit_message>
[feat][contianer][Add redis docker compose file, kong gateway docker compse file]
</commit_message>
<xml_diff>
--- a/Dev-Ops/Documents/System_Design.xlsx
+++ b/Dev-Ops/Documents/System_Design.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\my-work-space\My-Documents\Dev-Ops\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA39FF01-280B-41E6-98A1-54CD7618CCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13530" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -13,7 +19,7 @@
     <sheet name="3.Architechture" sheetId="22" r:id="rId4"/>
     <sheet name="4.Microservice" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -28,7 +34,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">-  là kiến trúc xây dựng hệ thống theo hướng phân tán, chia nhỏ hệ thống thành các micro service phục vụ cho các mục đích bussiness domain khác nhau
 - Nổi bật là :
@@ -40,7 +46,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> + Gateway
    + Discory service
@@ -56,7 +62,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">- </t>
     </r>
@@ -66,7 +72,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>Ưu</t>
     </r>
@@ -75,7 +81,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: Dễ mở rộng quy mô, nhờ độc lập nên khả năng chống chịu lỗi tốt (không bị ảnh hưởng khi bất kỳ service nào gặp lỗi), Dễ tích hợp công nghệ mới giảm phụ thuộc khi nâng cấp công nghệ giữa các module, Dễ dàng khi triển khai độc lập từng module
 - </t>
@@ -86,7 +92,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>Nhược</t>
     </r>
@@ -95,7 +101,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>: Giao tiếp giữa các các service tốn nhiều chi phí và có thể phức tạp hơn. Triển khai toàn hệ thống sẽ phức tạp hơn, cần tính toán về mặt tài nguyên để phân chia phù hợp cho các microservice,</t>
     </r>
@@ -144,7 +150,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>Encoding</t>
     </r>
@@ -153,7 +159,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: chuyển đổi dữ liệu, với mỗi dữ liệu đầu vào sẽ trả về dữ liệu đầu ra tương ứng
 Ví dụ: public String reverse(String input) - nhận một chuỗi và trả kết quả là chuỗi ngược lại.
@@ -165,7 +171,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>Encrypting</t>
     </r>
@@ -174,7 +180,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: là một kiểu encoding đặc biệt mà trong đó, để nhận được kết quả đầu ra, ta cần truyền một đầu vào và một khóa mật mã. Mã này cho phép kết quả sau khi biến đổi có thể xử lý ngược lại để nhận được kết quả đầu nếu ta biết được khóa mật mã và cách thức giải mật:
 (input, key_input) =&gt; output . Từ đó, người giải mã có thể dịch ngược lại với hàm (output, key_output) =&gt; input
@@ -187,7 +193,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>Hashing</t>
     </r>
@@ -196,7 +202,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>: là một kiểu encrypting nhưng chỉ có một chiều. Tức là tồn tại hàm (input) =&gt; output nhưng không có hàm (output) =&gt; input. Tuy nhiên, hashing vẫn tồn tại hàm cho phép kiểm tra 2 input có ra kết quả tương tự nhau không. Tức là nếu có hàm (input, key_input) =&gt; output , thì cũng cần có hàm (input1, input2) =&gt; boolean để so sánh giữa hai input.
 Đôi khi, hashing còn thêm một một giá trị ngẫu nhiên trong quá trình mã hóa đầu vào (input, salt) =&gt; output. Việc thêm salt vào trong hashing function khiến quá trình giải ngược lại mật mã trở nên khó khăn hơn rất nhiều (không thể đơn giản sử dụng một reverse hashing function để tìm được mật khẩu ban đầu)</t>
@@ -211,7 +217,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">1. request sẽ được được gửi đến Dispatcher Servlet (Front Controller)
 2. Dispatch Server sử dụng handler mapping để t controller xử lý request
@@ -228,7 +234,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Trong Mô hình MVC thì:
 </t>
@@ -238,7 +244,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 Model: là các file POJO, Service, DAO thực hiện truy cập database, xử lý business
@@ -381,7 +387,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Kafka là một nền tảng truyền dữ liệu phân tán (distributed messaging system). Kafka sử dụng mô hình truyền thông public-subscribe, bên public dữ liệu được gọi là producer bên subscribe </t>
     </r>
@@ -391,7 +397,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>nhận dữ liệu theo topic</t>
     </r>
@@ -400,7 +406,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> được gọi là consumer. Kafka có khả năng truyền một lượng lớn dữ liệu trong thời gian thực, trong trường hợp bên nhận </t>
     </r>
@@ -410,7 +416,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>chưa nhận dữ liệu</t>
     </r>
@@ -419,7 +425,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> vẫn được </t>
     </r>
@@ -429,7 +435,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>lưu trữ lại</t>
     </r>
@@ -438,7 +444,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> để bảo đảm an toàn về mặt dữ liệu.
 Nếu hệ thống của bạn không cần lưu trữ message, ưu tiên cho việc đòi hỏi sự đảm bảo rằng các consumer đều nhận được message và duy nhất bên cạnh độ ưu tiên của từng message thì dạng messaging truyền thống như RabbitMQ sẽ thực sự hữu dụng.
@@ -450,7 +456,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> đòi hỏi về mặt lưu trữ</t>
     </r>
@@ -459,7 +465,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> và</t>
     </r>
@@ -469,7 +475,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> tốc độ truyền tải message</t>
     </r>
@@ -478,7 +484,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">. Consumer muốn lựa chọn số lượng message mình cần, có thể lấy theo thứ tự hoặc muốn lấy từ lúc bắt đầu, </t>
     </r>
@@ -488,7 +494,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>một consumer có thể nhận đi nhận lại nhiều lần message</t>
     </r>
@@ -497,7 +503,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> đấy. Lúc này đây, hệ thông messaging dạng pipeline như Kafka sẽ được tin dùng. Có thể kể đến một số user cases như: Stream Processing, Event sourcing,..</t>
     </r>
@@ -511,7 +517,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Các tính năng đặc trưng của thành phần trong hệ thống Map
 Có 2 class thực thi trực tiếp Map interface bao gồm
@@ -523,7 +529,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>Hashtable</t>
     </r>
@@ -532,7 +538,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: Không chứa giá trị null, hỗ trợ đồng bộ nhưng đã lỗi thời.
 </t>
@@ -543,7 +549,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>Hashmap</t>
     </r>
@@ -552,7 +558,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: Cho phép chứa giá trị null, không hỗ trợ đồng bộ, với đặc điểm đặc trưng là thứ tự lặp (iteration order) không theo một quy tắc nào (random).
 Class </t>
@@ -563,7 +569,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">TreeMap </t>
     </r>
@@ -572,7 +578,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">thực thi gián tiếp qua các interface mở rộng của interface Map, với đặc điểm đặc trưng là tự động sắp xếp giá trị (theo thứ tự tự nhiên).
 Class </t>
@@ -583,7 +589,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">LinkedHashMap </t>
     </r>
@@ -592,7 +598,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>extends từ class HashMap, với đặc điểm đặc trưng là thứ tự lặp là thứ tự ban đầu của các Entry (thứ tự thêm vào).
 HashMap lưu trữ dữ liệu</t>
@@ -603,7 +609,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> theo các cặp</t>
     </r>
@@ -612,7 +618,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (viết tắt là K-V). Mỗi cặp được lưu trữ trong 1 đối tượng gọi là </t>
     </r>
@@ -622,7 +628,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>Entry</t>
     </r>
@@ -631,7 +637,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>, và Entry này được</t>
     </r>
@@ -641,7 +647,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> lưu trong một table tuân theo nguyên tắc Hashing</t>
     </r>
@@ -663,7 +669,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Advantages</t>
@@ -673,7 +679,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 
@@ -689,7 +695,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Disadvantages</t>
@@ -699,7 +705,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 
@@ -719,7 +725,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Fundamental</t>
@@ -729,7 +735,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 
@@ -746,7 +752,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Database Challenges
@@ -757,7 +763,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>building distributed applications that require low latency (độ trễ thấp) and scalability(khả năng mở rộng)
@@ -779,7 +785,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Lazy caching
@@ -790,7 +796,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>to populate the cache only when an object is actually requested by the application</t>
@@ -801,7 +807,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -812,7 +818,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> should apply a lazy caching strategy anywhere in your app where you have data that is going to be read often, but written infrequently</t>
@@ -825,7 +831,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Write-through
@@ -836,7 +842,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>the cache is updated in real time when the database is updated</t>
@@ -847,7 +853,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -858,7 +864,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>It avoids cache misses, which can help the application perform better and feel snappier</t>
@@ -883,7 +889,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Inmemory Cache
@@ -894,7 +900,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>- In-memory caching is a type of caching that involves storing data in the computer’s RAM (Random Access Memory) instead of in a database or on disk
@@ -908,7 +914,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Client-side Cache
@@ -919,7 +925,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>- Client-side caching is a type of caching that involves storing data on the client’s device, such as a web browser. This type of caching is useful for web applications that require frequent access to static resources, such as images and JavaScript files
@@ -933,7 +939,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Distributed Cache
@@ -944,7 +950,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">- that involves storing data across multiple servers or nodes in a network
@@ -958,7 +964,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Use case</t>
@@ -968,7 +974,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> :
@@ -982,7 +988,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Shared Storage</t>
@@ -992,7 +998,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -1012,7 +1018,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Local Caches:
@@ -1023,7 +1029,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> - A local cache stores your frequently used data within your application
@@ -1039,7 +1045,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Remote caches
@@ -1050,7 +1056,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> -  Remote caches are stored on dedicated servers(servers chuyên dụng) and typically built upon key/value NoSQL stores such as Redis and Memcached. They provide hundreds of thousands to up-to a million requests per second per cache node</t>
@@ -1072,7 +1078,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Cache-Aside (Cache Service  implements in Spring)
@@ -1083,7 +1089,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">- In this strategy, the application is responsible for managing the cache. When data is requested, the application checks the cache first. If the data is not in the cache, it is retrieved from the database and stored in the cache for future use. 
@@ -1095,7 +1101,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Pros</t>
@@ -1105,7 +1111,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">: 
@@ -1119,7 +1125,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Cons</t>
@@ -1129,7 +1135,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">: 
@@ -1142,7 +1148,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>higher latency</t>
@@ -1152,7 +1158,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">(độ trễ cao) whenever there's a </t>
@@ -1163,7 +1169,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>cache miss</t>
@@ -1173,7 +1179,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, as the data has to be retrieved from the database and then loaded into the cache.
@@ -1185,7 +1191,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>When to use</t>
@@ -1195,7 +1201,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">: 
@@ -1207,7 +1213,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>cache misses are rare(hiếm khi xảy ra)</t>
@@ -1217,7 +1223,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, and </t>
@@ -1228,7 +1234,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>the cost of a cache miss is not overly detrimental to performance</t>
@@ -1238,7 +1244,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
@@ -1251,7 +1257,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Read-Through (CacheAble annotation in Spring)
@@ -1262,7 +1268,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">- The cache is used as the primary data source. When data is requested, the cache is checked first. If the data is not in the cache, it is retrieved from the database and stored in the cache for future use. 
@@ -1275,7 +1281,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>if there is a cache hit</t>
@@ -1285,7 +1291,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>, the</t>
@@ -1296,7 +1302,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> application retrieves the data directly from the cache</t>
@@ -1306,7 +1312,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, just like in the cache-aside strategy. 
@@ -1318,7 +1324,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>in case of a cache miss</t>
@@ -1328,7 +1334,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>, the</t>
@@ -1339,7 +1345,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> cache server fetches data from the database</t>
@@ -1349,7 +1355,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, </t>
@@ -1360,7 +1366,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>not the application</t>
@@ -1370,7 +1376,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">. The Read-Through strategy places the responsibility of loading the data into the cache on the cache itself.
@@ -1389,7 +1395,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>have complex data loading requirements</t>
@@ -1399,7 +1405,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, and you want to maintain a clean separation between the cache and the client
@@ -1414,7 +1420,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Write-Through </t>
@@ -1424,7 +1430,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">(The Write-Through cache strategy stands out for its emphasis on </t>
@@ -1435,7 +1441,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>data consistency</t>
@@ -1445,7 +1451,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
@@ -1456,7 +1462,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -1467,7 +1473,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">In this strategy, data is written to both the cache and the database </t>
@@ -1478,7 +1484,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>at the same time</t>
@@ -1488,7 +1494,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">. 
@@ -1500,7 +1506,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>simultaneously(đồng thời)</t>
@@ -1510,7 +1516,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>. This ensures that the cache always contains up-to-date data, but it can slow down write operations
@@ -1531,7 +1537,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Write-Behind
@@ -1542,7 +1548,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">- In this strategy, data is </t>
@@ -1553,7 +1559,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>written to the cache first</t>
@@ -1563,7 +1569,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> and then to the </t>
@@ -1574,7 +1580,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>database at a later time</t>
@@ -1584,7 +1590,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">. 
@@ -1596,7 +1602,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>operations to be faster</t>
@@ -1606,7 +1612,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">, but it can lead to data </t>
@@ -1617,7 +1623,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>inconsistencies</t>
@@ -1627,7 +1633,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> if the cache is not properly managed.</t>
@@ -1640,7 +1646,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Write Around Cache
@@ -1651,7 +1657,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>write to the database but in this case you don’t update the cache. So data is written directly to the storage, bypassing the cache</t>
@@ -1664,7 +1670,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Write Back Cache
@@ -1675,7 +1681,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Firstly flush(xóa) the data from the cache, and then write the data to the cache alone. Once the data is updated in the cache, mark the data as modified, which means the data needs to be updated in DB later. Later an async(bất đồng bộ) job will be performed and at regular intervals, the modified data from the cache will be read to update the database with the corresponding values</t>
@@ -1694,7 +1700,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Cache Replacement
@@ -1705,7 +1711,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -1719,7 +1725,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1729,7 +1735,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>The cache in your system can be full at any point in time. So, we need to use some algorithm or strategy to remove the data from the cache, and we need to load other data that has more probability to be accessed in the future. To make this decision we can use some cache eviction policy. Let’s discuss some cache eviction policies one by one…</t>
@@ -1742,7 +1748,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1755,7 +1761,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>LRU (Least Recently Used)</t>
@@ -1779,7 +1785,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Calculate the cache hit rate:
@@ -1792,7 +1798,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>A high hit rate indicates that your caching strategy is effective in reducing the load on the backend data store</t>
@@ -1802,7 +1808,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>. 
@@ -1815,7 +1821,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Analyze cache eviction rate:
@@ -1828,7 +1834,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>A high eviction rate can indicate that the cache expiration time is too short or the cache size is too small</t>
@@ -1838,7 +1844,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
@@ -1850,7 +1856,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Monitor data consistency:
@@ -1862,7 +1868,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Data consistency is critical in caching.</t>
@@ -1872,7 +1878,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 
@@ -1886,7 +1892,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Determine the right cache expiration time:
@@ -1899,7 +1905,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>A longer cache expiration time can improve the cache hit rate but increase the risk of stale data</t>
@@ -1909,7 +1915,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>. 
@@ -1925,7 +1931,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1936,7 +1942,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>@EnableCaching</t>
@@ -1946,7 +1952,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">   apply this annotation at the main class (starter class) of our application in order to tell Spring Container 
@@ -1959,7 +1965,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1970,7 +1976,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>@Cacheable</t>
@@ -1980,7 +1986,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 
@@ -1996,7 +2002,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -2007,7 +2013,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>@CachePut</t>
@@ -2017,7 +2023,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> update data in the Redis Cache while there is any update of data in DB. 
@@ -2030,7 +2036,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -2041,7 +2047,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>@CacheEvict</t>
@@ -2051,7 +2057,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> remove the data in the Redis Cache while there is any removal of data in DB. 
@@ -2064,7 +2070,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -2075,7 +2081,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">@Caching </t>
@@ -2085,7 +2091,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>multiple annotations of the same type for caching a method</t>
@@ -2097,7 +2103,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -2108,7 +2114,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">@CacheConfig </t>
@@ -2118,7 +2124,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>we can streamline some of the cache configuration into a single place at the class level, so that we don’t have to declare things multiple times</t>
@@ -2472,14 +2478,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-  </numFmts>
-  <fonts count="31">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2488,25 +2488,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF954F72"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2514,27 +2521,27 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2542,7 +2549,7 @@
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2550,7 +2557,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2558,143 +2565,21 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2704,7 +2589,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2712,10 +2597,10 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2734,182 +2619,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2917,245 +2628,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3163,37 +2643,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="33" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="23" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="48" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3202,103 +2676,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="48" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="48" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -3314,13 +2765,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Ảnh 2"/>
+        <xdr:cNvPr id="3" name="Ảnh 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3352,13 +2809,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Ảnh 3"/>
+        <xdr:cNvPr id="4" name="Ảnh 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3390,13 +2853,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Ảnh 4"/>
+        <xdr:cNvPr id="5" name="Ảnh 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3417,7 +2886,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -3433,13 +2902,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3711,175 +3186,175 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView topLeftCell="B9" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="12.75" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.14" style="23"/>
-    <col min="2" max="2" width="39.5733333333333" style="23" customWidth="1"/>
-    <col min="3" max="3" width="95.5733333333333" style="23" customWidth="1"/>
-    <col min="4" max="4" width="60.7133333333333" style="23" customWidth="1"/>
-    <col min="5" max="5" width="58.8533333333333" style="23" customWidth="1"/>
-    <col min="6" max="6" width="50" style="23" customWidth="1"/>
-    <col min="7" max="7" width="49.7133333333333" style="23" customWidth="1"/>
-    <col min="8" max="16384" width="9.14" style="23"/>
+    <col min="1" max="1" width="9.140625" style="19"/>
+    <col min="2" max="2" width="39.5703125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="95.5703125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="60.7109375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="58.85546875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="50" style="19" customWidth="1"/>
+    <col min="7" max="7" width="49.7109375" style="19" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" ht="76.5" spans="1:3">
-      <c r="A1" s="23">
+    <row r="1" spans="1:7" ht="90">
+      <c r="A1" s="19">
         <v>1</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="63.75" spans="1:3">
-      <c r="A2" s="23">
+    <row r="2" spans="1:7" ht="75">
+      <c r="A2" s="19">
         <v>2</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="38.25" spans="1:3">
-      <c r="A3" s="23">
+    <row r="3" spans="1:7" ht="45">
+      <c r="A3" s="19">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="38.25" spans="1:3">
-      <c r="A4" s="23">
+    <row r="4" spans="1:7" ht="45">
+      <c r="A4" s="19">
         <v>4</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="178.5" spans="1:3">
-      <c r="A5" s="23">
+    <row r="5" spans="1:7" ht="240">
+      <c r="A5" s="19">
         <v>5</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="25.5" spans="1:3">
-      <c r="A6" s="23">
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6" s="19">
         <v>6</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="229.5" spans="1:3">
-      <c r="A7" s="23">
+    <row r="7" spans="1:7" ht="300">
+      <c r="A7" s="19">
         <v>7</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" ht="245.25" customHeight="1" spans="1:3">
-      <c r="A8" s="23">
+    <row r="8" spans="1:7" ht="245.25" customHeight="1">
+      <c r="A8" s="19">
         <v>8</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="223.5" customHeight="1" spans="1:3">
-      <c r="A9" s="23">
+    <row r="9" spans="1:7" ht="223.5" customHeight="1">
+      <c r="A9" s="19">
         <v>9</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" ht="204" spans="1:4">
-      <c r="A10" s="23">
+    <row r="10" spans="1:7" ht="300">
+      <c r="A10" s="19">
         <v>10</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" ht="25.5" spans="2:3">
-      <c r="B11" s="23" t="s">
+    <row r="11" spans="1:7" ht="30">
+      <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" ht="102" spans="2:3">
-      <c r="B12" s="23" t="s">
+    <row r="12" spans="1:7" ht="150">
+      <c r="B12" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" ht="140.25" spans="2:3">
-      <c r="B13" s="23" t="s">
+    <row r="13" spans="1:7" ht="180">
+      <c r="B13" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" ht="288.75" customHeight="1" spans="2:7">
-      <c r="B14" s="23" t="s">
+    <row r="14" spans="1:7" ht="288.75" customHeight="1">
+      <c r="B14" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="20" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -3892,589 +3367,586 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" ht="38.25" spans="2:3">
-      <c r="B15" s="23" t="s">
+    <row r="15" spans="1:7" ht="60">
+      <c r="B15" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" ht="240.75" customHeight="1" spans="2:2">
-      <c r="B16" s="23" t="s">
+    <row r="16" spans="1:7" ht="240.75" customHeight="1">
+      <c r="B16" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" ht="153" spans="2:3">
-      <c r="B17" s="23" t="s">
+    <row r="17" spans="2:3" ht="180">
+      <c r="B17" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" ht="153" spans="2:3">
-      <c r="B18" s="23" t="s">
+    <row r="18" spans="2:3" ht="180">
+      <c r="B18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="20" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId2" display="https://topdev.vn/blog/trien-khai-ci-cd-voi-gitlab/"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.14" customWidth="1"/>
-    <col min="2" max="2" width="110.853333333333" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="110.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="89.25" spans="1:2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:2" ht="105">
+      <c r="A1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" ht="89.25" spans="1:2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="1:2" ht="105">
+      <c r="A2" s="26"/>
+      <c r="B2" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" ht="102" spans="1:2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="1:2" ht="135">
+      <c r="A3" s="26"/>
+      <c r="B3" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" ht="63.75" spans="1:2">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:2" ht="90">
+      <c r="A4" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" ht="63.75" spans="1:2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="18" t="s">
+    <row r="5" spans="1:2" ht="75">
+      <c r="A5" s="26"/>
+      <c r="B5" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" ht="38.25" spans="1:2">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:2" ht="60">
+      <c r="A7" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" ht="38.25" spans="1:2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="18" t="s">
+    <row r="8" spans="1:2" ht="45">
+      <c r="A8" s="26"/>
+      <c r="B8" s="16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="16" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" ht="51" spans="1:2">
-      <c r="A12" s="16" t="s">
+    <row r="12" spans="1:2" ht="60">
+      <c r="A12" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" ht="63.75" spans="1:2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="18" t="s">
+    <row r="13" spans="1:2" ht="90">
+      <c r="A13" s="26"/>
+      <c r="B13" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" ht="127.5" spans="1:2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="18" t="s">
+    <row r="14" spans="1:2" ht="165">
+      <c r="A14" s="26"/>
+      <c r="B14" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="18" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="16" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" ht="102" spans="1:2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="18" t="s">
+    <row r="17" spans="1:2" ht="120">
+      <c r="A17" s="26"/>
+      <c r="B17" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" ht="38.25" spans="1:2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="18" t="s">
+    <row r="18" spans="1:2" ht="60">
+      <c r="A18" s="26"/>
+      <c r="B18" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="16"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" ht="165.75" spans="1:2">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:2" ht="195">
+      <c r="A21" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" ht="242.25" spans="1:2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="18" t="s">
+    <row r="22" spans="1:2" ht="300">
+      <c r="A22" s="27"/>
+      <c r="B22" s="16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" ht="153" spans="1:2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="18" t="s">
+    <row r="23" spans="1:2" ht="195">
+      <c r="A23" s="27"/>
+      <c r="B23" s="16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" ht="38.25" spans="1:2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="18" t="s">
+    <row r="24" spans="1:2" ht="45">
+      <c r="A24" s="27"/>
+      <c r="B24" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" ht="25.5" spans="1:2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="18" t="s">
+    <row r="25" spans="1:2" ht="45">
+      <c r="A25" s="27"/>
+      <c r="B25" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" ht="51" spans="1:2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="18" t="s">
+    <row r="26" spans="1:2" ht="75">
+      <c r="A26" s="27"/>
+      <c r="B26" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="18" t="s">
+      <c r="A27" s="27"/>
+      <c r="B27" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="19" t="s">
+      <c r="A28" s="27"/>
+      <c r="B28" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" ht="38.25" spans="1:2">
-      <c r="A29" s="21" t="s">
+    <row r="29" spans="1:2" ht="45">
+      <c r="A29" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="16" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="16"/>
-      <c r="B30" s="18" t="s">
+      <c r="A30" s="26"/>
+      <c r="B30" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="16"/>
-      <c r="B31" s="18" t="s">
+      <c r="A31" s="26"/>
+      <c r="B31" s="16" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="16"/>
-      <c r="B32" s="18" t="s">
+      <c r="A32" s="26"/>
+      <c r="B32" s="16" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="16"/>
-      <c r="B33" s="18" t="s">
+      <c r="A33" s="26"/>
+      <c r="B33" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" ht="51" spans="1:2">
-      <c r="A34" s="20" t="s">
+    <row r="34" spans="1:2" ht="75">
+      <c r="A34" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" ht="38.25" spans="1:2">
-      <c r="A35" s="16"/>
-      <c r="B35" s="17" t="s">
+    <row r="35" spans="1:2" ht="60">
+      <c r="A35" s="26"/>
+      <c r="B35" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" ht="51" spans="1:2">
-      <c r="A36" s="16"/>
-      <c r="B36" s="17" t="s">
+    <row r="36" spans="1:2" ht="75">
+      <c r="A36" s="26"/>
+      <c r="B36" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" ht="51" spans="1:2">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17" t="s">
+    <row r="37" spans="1:2" ht="75">
+      <c r="A37" s="26"/>
+      <c r="B37" s="15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" ht="25.5" spans="1:2">
-      <c r="A38" s="16" t="s">
+    <row r="38" spans="1:2" ht="45">
+      <c r="A38" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="39" ht="76.5" spans="1:2">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17" t="s">
+    <row r="39" spans="1:2" ht="90">
+      <c r="A39" s="26"/>
+      <c r="B39" s="15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" ht="25.5" spans="1:2">
-      <c r="A40" s="16"/>
-      <c r="B40" s="17" t="s">
+    <row r="40" spans="1:2" ht="30">
+      <c r="A40" s="26"/>
+      <c r="B40" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="41" ht="25.5" spans="1:2">
-      <c r="A41" s="16"/>
-      <c r="B41" s="17" t="s">
+    <row r="41" spans="1:2" ht="30">
+      <c r="A41" s="26"/>
+      <c r="B41" s="15" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="16"/>
-      <c r="B42" s="17" t="s">
+      <c r="A42" s="26"/>
+      <c r="B42" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" ht="25.5" spans="1:2">
-      <c r="A43" s="16"/>
-      <c r="B43" s="17" t="s">
+    <row r="43" spans="1:2" ht="30">
+      <c r="A43" s="26"/>
+      <c r="B43" s="15" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="16"/>
-      <c r="B44" s="17"/>
-    </row>
-    <row r="45" ht="25.5" spans="1:2">
-      <c r="A45" s="16" t="s">
+      <c r="A44" s="14"/>
+      <c r="B44" s="15"/>
+    </row>
+    <row r="45" spans="1:2" ht="30">
+      <c r="A45" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="18" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A43"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A20"/>
     <mergeCell ref="A21:A28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A43"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B45" r:id="rId2" display="https://developer.redis.com/develop/java/redis-and-spring-course/lesson_9&#10;https://www.bezkoder.com/spring-boot-redis-cache-example/"/>
+    <hyperlink ref="B45" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="55.8533333333333" style="8" customWidth="1"/>
-    <col min="2" max="2" width="54.14" style="9" customWidth="1"/>
-    <col min="3" max="3" width="101.713333333333" style="10" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="101.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" spans="1:1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" ht="12.75" spans="1:3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
-    </row>
-    <row r="3" ht="12.75" spans="1:2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-    </row>
-    <row r="4" ht="12.75" spans="1:2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-    </row>
-    <row r="5" ht="12.75" spans="1:2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-    </row>
-    <row r="6" ht="12.75" spans="1:2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-    </row>
-    <row r="7" ht="12.75" spans="1:2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-    </row>
-    <row r="8" ht="12.75" spans="1:2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-    </row>
-    <row r="9" ht="12.75" spans="1:2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-    </row>
-    <row r="10" ht="12.75" spans="1:2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-    </row>
-    <row r="11" ht="12.75" spans="1:2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-    </row>
-    <row r="12" ht="12.75" spans="1:2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-    </row>
-    <row r="13" ht="12.75" spans="1:2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-    </row>
-    <row r="14" ht="12.75" spans="1:2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-    </row>
-    <row r="15" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-    </row>
-    <row r="16" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-    </row>
-    <row r="17" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-    </row>
-    <row r="18" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-    </row>
-    <row r="19" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-    </row>
-    <row r="20" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-    </row>
-    <row r="21" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-    </row>
-    <row r="22" ht="17.25" spans="1:2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" ht="17.25" spans="1:2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-    </row>
-    <row r="24" ht="17.25" spans="1:2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="14"/>
-    </row>
-    <row r="26" ht="17.25" spans="1:2">
-      <c r="A26" s="11" t="s">
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="29"/>
+      <c r="B4" s="30"/>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+    </row>
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30"/>
+    </row>
+    <row r="9" spans="1:3" ht="15">
+      <c r="A9" s="29"/>
+      <c r="B9" s="30"/>
+    </row>
+    <row r="10" spans="1:3" ht="15">
+      <c r="A10" s="29"/>
+      <c r="B10" s="30"/>
+    </row>
+    <row r="11" spans="1:3" ht="15">
+      <c r="A11" s="29"/>
+      <c r="B11" s="30"/>
+    </row>
+    <row r="12" spans="1:3" ht="15">
+      <c r="A12" s="29"/>
+      <c r="B12" s="30"/>
+    </row>
+    <row r="13" spans="1:3" ht="15">
+      <c r="A13" s="29"/>
+      <c r="B13" s="30"/>
+    </row>
+    <row r="14" spans="1:3" ht="15">
+      <c r="A14" s="29"/>
+      <c r="B14" s="30"/>
+    </row>
+    <row r="15" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+    </row>
+    <row r="16" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A16" s="29"/>
+      <c r="B16" s="30"/>
+    </row>
+    <row r="17" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
+    </row>
+    <row r="18" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
+    </row>
+    <row r="19" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A19" s="29"/>
+      <c r="B19" s="30"/>
+    </row>
+    <row r="20" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A20" s="29"/>
+      <c r="B20" s="30"/>
+    </row>
+    <row r="21" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
+    </row>
+    <row r="22" spans="1:3" ht="18.75">
+      <c r="A22" s="29"/>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:3" ht="18.75">
+      <c r="A23" s="29"/>
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="1:3" ht="18.75">
+      <c r="A24" s="29"/>
+      <c r="B24" s="12"/>
+    </row>
+    <row r="26" spans="1:3" ht="18.75">
+      <c r="A26" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" ht="17.25" spans="1:2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="9" t="s">
+    <row r="27" spans="1:3" ht="18.75">
+      <c r="A27" s="29"/>
+      <c r="B27" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" ht="17.25" spans="1:2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="9" t="s">
+    <row r="28" spans="1:3" ht="18.75">
+      <c r="A28" s="29"/>
+      <c r="B28" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="11"/>
-    </row>
-    <row r="30" ht="12.75" spans="1:3">
-      <c r="A30" s="11" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" ht="15">
+      <c r="A30" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" ht="12.75" spans="1:3">
-      <c r="A31" s="11"/>
-      <c r="C31" s="10" t="s">
+    <row r="31" spans="1:3" ht="15">
+      <c r="A31" s="29"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="32" ht="12.75" spans="1:3">
-      <c r="A32" s="11"/>
-      <c r="C32" s="10" t="s">
+    <row r="32" spans="1:3" ht="15">
+      <c r="A32" s="29"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" ht="12.75" spans="1:3">
-      <c r="A33" s="11"/>
-      <c r="C33" s="10" t="s">
+    <row r="33" spans="1:3" ht="15">
+      <c r="A33" s="29"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="35" ht="114.75" spans="1:3">
-      <c r="A35" s="11" t="s">
+    <row r="35" spans="1:3" ht="165">
+      <c r="A35" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="25" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="36" ht="89.25" spans="1:3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="9" t="s">
+    <row r="36" spans="1:3" ht="105">
+      <c r="A36" s="29"/>
+      <c r="B36" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="25" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="37" ht="76.5" spans="1:3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="9" t="s">
+    <row r="37" spans="1:3" ht="105">
+      <c r="A37" s="29"/>
+      <c r="B37" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="13" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="38" ht="51" spans="1:3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="9" t="s">
+    <row r="38" spans="1:3" ht="60">
+      <c r="A38" s="29"/>
+      <c r="B38" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="11" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="9" t="s">
         <v>113</v>
       </c>
     </row>
@@ -4489,38 +3961,36 @@
     <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32" style="1" customWidth="1"/>
     <col min="2" max="2" width="109" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="127.5" spans="1:3">
+    <row r="1" spans="1:3" ht="150">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="24" t="s">
         <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" ht="200.25" customHeight="1" spans="1:2">
+    <row r="2" spans="1:3" ht="200.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>117</v>
       </c>
@@ -4528,7 +3998,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" ht="102" spans="1:2">
+    <row r="3" spans="1:3" ht="120">
       <c r="A3" s="1" t="s">
         <v>119</v>
       </c>
@@ -4536,15 +4006,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" ht="25.5" spans="1:2">
+    <row r="4" spans="1:3" ht="45">
       <c r="A4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="24" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" ht="25.5" spans="1:2">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" s="1" t="s">
         <v>123</v>
       </c>
@@ -4552,12 +4022,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" ht="38.25" spans="1:1">
+    <row r="6" spans="1:3" ht="45">
       <c r="A6" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" ht="38.25" spans="1:2">
+    <row r="7" spans="1:3" ht="45">
       <c r="A7" s="1" t="s">
         <v>126</v>
       </c>
@@ -4565,7 +4035,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" ht="114.75" spans="1:2">
+    <row r="8" spans="1:3" ht="150">
       <c r="A8" s="1" t="s">
         <v>128</v>
       </c>
@@ -4573,7 +4043,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" ht="51" spans="1:2">
+    <row r="12" spans="1:3" ht="60">
       <c r="A12" s="1" t="s">
         <v>130</v>
       </c>
@@ -4581,7 +4051,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" ht="51" spans="1:2">
+    <row r="13" spans="1:3" ht="60">
       <c r="A13" s="1" t="s">
         <v>132</v>
       </c>
@@ -4589,7 +4059,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" ht="89.25" spans="1:2">
+    <row r="14" spans="1:3" ht="120">
       <c r="A14" s="1" t="s">
         <v>134</v>
       </c>
@@ -4597,7 +4067,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" ht="102" spans="1:2">
+    <row r="15" spans="1:3" ht="120">
       <c r="A15" s="1" t="s">
         <v>136</v>
       </c>
@@ -4605,7 +4075,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>138</v>
       </c>
@@ -4613,7 +4083,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" ht="178.5" spans="1:2">
+    <row r="17" spans="1:2" ht="225">
       <c r="A17" s="1" t="s">
         <v>140</v>
       </c>
@@ -4621,7 +4091,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" ht="25.5" spans="1:2">
+    <row r="18" spans="1:2" ht="30">
       <c r="A18" s="1" t="s">
         <v>142</v>
       </c>
@@ -4629,7 +4099,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" ht="280.5" spans="1:2">
+    <row r="19" spans="1:2" ht="345">
       <c r="A19" s="1" t="s">
         <v>144</v>
       </c>
@@ -4637,25 +4107,25 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="1:2">
       <c r="B23" s="4"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>149</v>
       </c>
@@ -4668,7 +4138,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" ht="38.25" spans="1:2">
+    <row r="33" spans="1:2" ht="45">
       <c r="A33" s="1" t="s">
         <v>152</v>
       </c>
@@ -4676,7 +4146,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" ht="114.75" spans="1:2">
+    <row r="34" spans="1:2" ht="135">
       <c r="A34" s="1" t="s">
         <v>154</v>
       </c>
@@ -4684,53 +4154,53 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="32" t="s">
         <v>165</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -4738,19 +4208,19 @@
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="5"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="5"/>
+      <c r="A56" s="32"/>
       <c r="B56" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="58" ht="25.5" spans="1:2">
-      <c r="A58" s="6" t="s">
+    <row r="58" spans="1:2" ht="30">
+      <c r="A58" s="33" t="s">
         <v>169</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -4758,38 +4228,38 @@
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="6"/>
-      <c r="B59" s="7" t="s">
+      <c r="A59" s="33"/>
+      <c r="B59" s="5" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="6"/>
-      <c r="B60" s="7" t="s">
+      <c r="A60" s="33"/>
+      <c r="B60" s="5" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="6"/>
-      <c r="B61" s="7" t="s">
+      <c r="A61" s="33"/>
+      <c r="B61" s="5" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="6"/>
-      <c r="B62" s="7" t="s">
+      <c r="A62" s="33"/>
+      <c r="B62" s="5" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="6"/>
-      <c r="B63" s="7" t="s">
+      <c r="A63" s="33"/>
+      <c r="B63" s="5" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="6"/>
-      <c r="B64" s="7" t="s">
+      <c r="A64" s="33"/>
+      <c r="B64" s="5" t="s">
         <v>176</v>
       </c>
     </row>
@@ -4799,9 +4269,8 @@
     <mergeCell ref="A58:A64"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" display="HƯỚNG DẪN CÁC BƯỚC PHÁT TRIỂN HỆ THỐNG MICROSERVICE VỚI DOCKER | CO-WELL Asia"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[feat][redis][Add redis docker compose]
</commit_message>
<xml_diff>
--- a/Dev-Ops/Documents/System_Design.xlsx
+++ b/Dev-Ops/Documents/System_Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\my-work-space\My-Documents\Dev-Ops\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA39FF01-280B-41E6-98A1-54CD7618CCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669D6527-754A-4F6D-9F57-0DADBB89541E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
   <si>
     <t>Kiến Trúc về Microservice</t>
   </si>
@@ -2134,10 +2134,6 @@
     <t xml:space="preserve">Redis </t>
   </si>
   <si>
-    <t>https://developer.redis.com/develop/java/redis-and-spring-course/lesson_9
-https://www.bezkoder.com/spring-boot-redis-cache-example/</t>
-  </si>
-  <si>
     <t>SYSTEM DESIGN</t>
   </si>
   <si>
@@ -2474,12 +2470,21 @@
   <si>
     <t>FallBack Techniques</t>
   </si>
+  <si>
+    <t>https://developer.redis.com/develop/java/redis-and-spring-course/lesson_9
+https://www.bezkoder.com/spring-boot-redis-cache-example/
+https://faun.pub/redis-master-slave-configuration-and-tested-in-spring-boot-3a68e7314b90
+https://www.vinsguru.com/category/redis/</t>
+  </si>
+  <si>
+    <t>REDIS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2599,6 +2604,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2635,7 +2648,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2704,14 +2717,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2727,6 +2740,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3421,10 +3437,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3434,7 +3450,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="105">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="15" t="s">
@@ -3442,19 +3458,19 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="105">
-      <c r="A2" s="26"/>
+      <c r="A2" s="27"/>
       <c r="B2" s="16" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="135">
-      <c r="A3" s="26"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="90">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -3462,19 +3478,19 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="75">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="26"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="16" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="60">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -3482,31 +3498,31 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="45">
-      <c r="A8" s="26"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="26"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="16" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="60">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -3514,55 +3530,55 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="90">
-      <c r="A13" s="26"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="165">
-      <c r="A14" s="26"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="26"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="16" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="26"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="16" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="120">
-      <c r="A17" s="26"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="60">
-      <c r="A18" s="26"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="26"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="17" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="195">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="28" t="s">
         <v>64</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -3570,49 +3586,49 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="300">
-      <c r="A22" s="27"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="195">
-      <c r="A23" s="27"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="27"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="16" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="45">
-      <c r="A25" s="27"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="75">
-      <c r="A26" s="27"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="27"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="27"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="45">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="26" t="s">
         <v>73</v>
       </c>
       <c r="B29" s="16" t="s">
@@ -3620,31 +3636,31 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="26"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="26"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="16" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="26"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="16" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="26"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="16" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="75">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="28" t="s">
         <v>79</v>
       </c>
       <c r="B34" s="15" t="s">
@@ -3652,25 +3668,25 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="60">
-      <c r="A35" s="26"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="75">
-      <c r="A36" s="26"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="75">
-      <c r="A37" s="26"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="15" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="45">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="27" t="s">
         <v>84</v>
       </c>
       <c r="B38" s="15" t="s">
@@ -3678,31 +3694,31 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="90">
-      <c r="A39" s="26"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="15" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30">
-      <c r="A40" s="26"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="15" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="30">
-      <c r="A41" s="26"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="15" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="26"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="15" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="30">
-      <c r="A43" s="26"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="15" t="s">
         <v>90</v>
       </c>
@@ -3711,16 +3727,27 @@
       <c r="A44" s="14"/>
       <c r="B44" s="15"/>
     </row>
-    <row r="45" spans="1:2" ht="30">
-      <c r="A45" s="14" t="s">
+    <row r="45" spans="1:2" ht="26.25" customHeight="1">
+      <c r="A45" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="34"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
+    </row>
+    <row r="47" spans="1:2" ht="60">
+      <c r="A47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="18" t="s">
-        <v>92</v>
+      <c r="B47" s="18" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A45:B46"/>
     <mergeCell ref="A29:A33"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="A38:A43"/>
@@ -3731,11 +3758,11 @@
     <mergeCell ref="A21:A28"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B45" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B47" r:id="rId1" display="https://developer.redis.com/develop/java/redis-and-spring-course/lesson_9_x000a_https://www.bezkoder.com/spring-boot-redis-cache-example/" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3756,7 +3783,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15">
@@ -3854,22 +3881,22 @@
     </row>
     <row r="26" spans="1:3" ht="18.75">
       <c r="A26" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18.75">
       <c r="A27" s="29"/>
       <c r="B27" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75">
       <c r="A28" s="29"/>
       <c r="B28" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -3877,77 +3904,77 @@
     </row>
     <row r="30" spans="1:3" ht="15">
       <c r="A30" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="C30" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15">
       <c r="A31" s="29"/>
       <c r="B31" s="31"/>
       <c r="C31" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15">
       <c r="A32" s="29"/>
       <c r="B32" s="31"/>
       <c r="C32" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15">
       <c r="A33" s="29"/>
       <c r="B33" s="31"/>
       <c r="C33" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="165">
       <c r="A35" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="C35" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="105">
       <c r="A36" s="29"/>
       <c r="B36" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="25" t="s">
         <v>107</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="105">
       <c r="A37" s="29"/>
       <c r="B37" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>109</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="60">
       <c r="A38" s="29"/>
       <c r="B38" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>111</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3981,140 +4008,140 @@
   <sheetData>
     <row r="1" spans="1:3" ht="150">
       <c r="A1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="200.25" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="120">
       <c r="A3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45">
       <c r="A4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>121</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
       <c r="A5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45">
       <c r="A6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45">
       <c r="A7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150">
       <c r="A8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60">
       <c r="A12" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60">
       <c r="A13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="120">
       <c r="A14" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="120">
       <c r="A15" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="225">
       <c r="A17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30">
       <c r="A18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="345">
       <c r="A19" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4122,145 +4149,145 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
       <c r="A33" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="135">
       <c r="A34" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="32"/>
       <c r="B55" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="32"/>
       <c r="B56" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30">
       <c r="A58" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="33"/>
       <c r="B59" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="33"/>
       <c r="B60" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="33"/>
       <c r="B61" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="33"/>
       <c r="B62" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="33"/>
       <c r="B63" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="33"/>
       <c r="B64" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>